<commit_message>
Update the daily log~
</commit_message>
<xml_diff>
--- a/daily log/工作日志.杨炜.3月份.xlsx
+++ b/daily log/工作日志.杨炜.3月份.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28710" windowHeight="13050" activeTab="2"/>
+    <workbookView windowWidth="28710" windowHeight="13050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="周计划" sheetId="1" r:id="rId1"/>
     <sheet name="第二周" sheetId="2" r:id="rId2"/>
     <sheet name="第三周" sheetId="3" r:id="rId3"/>
-    <sheet name="模板" sheetId="4" r:id="rId4"/>
+    <sheet name="第四周" sheetId="4" r:id="rId4"/>
+    <sheet name="模板" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120">
   <si>
     <t>下周计划</t>
   </si>
@@ -198,7 +199,7 @@
     <t>完成左侧栏部分</t>
   </si>
   <si>
-    <t>对资讯页进行切图</t>
+    <t>对媒体报道进行切图</t>
   </si>
   <si>
     <t>已完成</t>
@@ -210,7 +211,7 @@
     <t>对文件进行压缩处理</t>
   </si>
   <si>
-    <t>对资讯页进行web端全局分布</t>
+    <t>对媒体报道进行web端全局分布</t>
   </si>
   <si>
     <t>对图片进行sprite优化</t>
@@ -252,9 +253,15 @@
     <t>20日工作计划（周五）</t>
   </si>
   <si>
+    <t>初探jquery.parallax</t>
+  </si>
+  <si>
     <t>通过添加jQuery.fn.limit方法执行（待优化）</t>
   </si>
   <si>
+    <t>制作其他页面</t>
+  </si>
+  <si>
     <t>对max-width、min-width进行兼容</t>
   </si>
   <si>
@@ -267,7 +274,114 @@
     <t>使用无效</t>
   </si>
   <si>
+    <t>估摸是电脑原因，明天重启试试</t>
+  </si>
+  <si>
     <t>研究GetF5插件</t>
+  </si>
+  <si>
+    <t>制作媒体报道详情页</t>
+  </si>
+  <si>
+    <t>20日工作日志（周五）</t>
+  </si>
+  <si>
+    <t>23日工作计划（周一）</t>
+  </si>
+  <si>
+    <t>制作网站公告列表页</t>
+  </si>
+  <si>
+    <t>UI重新排列中</t>
+  </si>
+  <si>
+    <t>制作网站公告内页</t>
+  </si>
+  <si>
+    <t>学习连接VPN</t>
+  </si>
+  <si>
+    <t>成功连接，服务器太慢无法正常打开</t>
+  </si>
+  <si>
+    <t>制作动态信息列表页</t>
+  </si>
+  <si>
+    <t>制作动态信息内页</t>
+  </si>
+  <si>
+    <t>修正列表页jiathis分享url+summary</t>
+  </si>
+  <si>
+    <t>重置列表页页码格式</t>
+  </si>
+  <si>
+    <t>研究兼容css小三角-border-width</t>
+  </si>
+  <si>
+    <t>获取列表页默认图片</t>
+  </si>
+  <si>
+    <t>23日工作日志（周一）</t>
+  </si>
+  <si>
+    <t>24日工作计划（周二）</t>
+  </si>
+  <si>
+    <t>完成</t>
+  </si>
+  <si>
+    <t>制作新手指导页面</t>
+  </si>
+  <si>
+    <t>重新切图并应用</t>
+  </si>
+  <si>
+    <t>header-完成
+left-完成common+完成tag
+right-完成
+footer-完成</t>
+  </si>
+  <si>
+    <t>为了让结果能够更好的以块状形式很好的展现</t>
+  </si>
+  <si>
+    <t>替换左侧导航小三角为图片</t>
+  </si>
+  <si>
+    <t>暴力解决border-width兼容问题</t>
+  </si>
+  <si>
+    <t>完成响应式页面变换</t>
+  </si>
+  <si>
+    <t>媒体报道列表-完成
+媒体报道内容-完成
+动态信息列表-完成
+动态信息内容-完成
+网站公告列表-完成
+网站公告内容-完成</t>
+  </si>
+  <si>
+    <t>去除列表页中摘要的样式</t>
+  </si>
+  <si>
+    <t>设定好行高，并输出文本，已解决</t>
+  </si>
+  <si>
+    <t>直接清空即可，只需要标签存在，或者在显示文本的时候不添加标签，直接文字化输出</t>
+  </si>
+  <si>
+    <t>优化动态信息列表页中jiathis代码</t>
+  </si>
+  <si>
+    <t>减少部分</t>
+  </si>
+  <si>
+    <t>重复太多，试着减少，建议列表页不添加分享按钮</t>
+  </si>
+  <si>
+    <t>优化代码和图片</t>
   </si>
   <si>
     <t>日工作日志（周）</t>
@@ -282,9 +396,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -338,7 +452,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,14 +483,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -426,10 +534,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -456,10 +564,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -482,6 +590,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -500,13 +623,11 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -515,10 +636,40 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -528,10 +679,8 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -540,43 +689,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -632,6 +747,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -653,7 +783,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -675,16 +805,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -696,16 +829,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -723,19 +856,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -744,31 +880,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -789,7 +931,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1162,188 +1304,188 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="4.625" style="39" customWidth="1"/>
-    <col min="2" max="2" width="32.125" style="39" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="39" customWidth="1"/>
-    <col min="4" max="5" width="9" style="39"/>
-    <col min="6" max="6" width="15.625" style="39" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="39" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="39"/>
+    <col min="1" max="1" width="4.625" style="43" customWidth="1"/>
+    <col min="2" max="2" width="32.125" style="43" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="43" customWidth="1"/>
+    <col min="4" max="5" width="9" style="43"/>
+    <col min="6" max="6" width="15.625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="16.875" style="43" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="43"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.75" customHeight="1" spans="1:7">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
     <row r="2" ht="33" customHeight="1" spans="1:7">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
     </row>
     <row r="3" ht="16.5" spans="1:7">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="53" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:7">
-      <c r="A4" s="50">
+      <c r="A4" s="54">
         <v>1</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" ht="16.5" spans="1:7">
-      <c r="A5" s="50">
+      <c r="A5" s="54">
         <v>2</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
     </row>
     <row r="6" ht="16.5" spans="1:7">
-      <c r="A6" s="50">
+      <c r="A6" s="54">
         <v>3</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
     </row>
     <row r="7" ht="16.5" spans="1:7">
-      <c r="A7" s="50">
+      <c r="A7" s="54">
         <v>4</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
     </row>
     <row r="8" ht="16.5" spans="1:7">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="54"/>
+      <c r="B8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" ht="16.5" spans="1:7">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
     </row>
     <row r="10" ht="16.5" spans="1:7">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" ht="16.5" spans="1:7">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
     </row>
     <row r="12" ht="16.5" spans="1:7">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
     </row>
     <row r="13" ht="16.5" spans="1:7">
-      <c r="A13" s="50"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
     </row>
     <row r="14" ht="16.5" spans="1:7">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
     </row>
     <row r="15" ht="16.5" spans="1:7">
-      <c r="A15" s="50"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="56" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1366,14 +1508,14 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="19.125" style="39" customWidth="1"/>
+    <col min="2" max="2" width="19.125" style="43" customWidth="1"/>
     <col min="3" max="3" width="47.25" customWidth="1"/>
-    <col min="4" max="4" width="21" style="39" customWidth="1"/>
+    <col min="4" max="4" width="21" style="43" customWidth="1"/>
     <col min="5" max="5" width="6.75" customWidth="1"/>
     <col min="7" max="7" width="35.625" customWidth="1"/>
   </cols>
@@ -1414,154 +1556,154 @@
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" ht="28.5" spans="1:7">
-      <c r="A4" s="11"/>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="14">
+      <c r="E4" s="10"/>
+      <c r="F4" s="16">
         <v>2</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" ht="42.75" spans="1:7">
-      <c r="A5" s="11"/>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="14">
+      <c r="E5" s="10"/>
+      <c r="F5" s="16">
         <v>3</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" ht="17.25" spans="1:7">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="14">
+      <c r="A6" s="17"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16">
         <v>4</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" ht="17.25" spans="1:7">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="14">
+      <c r="A7" s="21"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="16">
         <v>5</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" ht="16.5" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14">
+      <c r="D8" s="15"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="16">
         <v>6</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" ht="28.5" spans="1:7">
-      <c r="A9" s="11"/>
-      <c r="B9" s="40" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14">
+      <c r="E9" s="10"/>
+      <c r="F9" s="16">
         <v>7</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" ht="16.5" spans="1:7">
-      <c r="A10" s="11"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="14">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="16">
         <v>8</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" ht="16.5" spans="1:7">
-      <c r="A11" s="11"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="16">
         <v>9</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" ht="17.25" spans="1:7">
-      <c r="A12" s="16"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="27">
+      <c r="A12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="29">
         <v>10</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" ht="17.25" spans="1:7">
-      <c r="A13" s="28"/>
-      <c r="B13" s="44" t="s">
+      <c r="A13" s="30"/>
+      <c r="B13" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1580,10 +1722,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59:G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1631,160 +1773,160 @@
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:7">
-      <c r="A4" s="11"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="14">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="16">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" ht="16.5" spans="1:7">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="14">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="16">
         <v>3</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" ht="17.25" spans="1:7">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="14">
+      <c r="A6" s="17"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16">
         <v>4</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" ht="17.25" spans="1:7">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="14">
+      <c r="A7" s="21"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="16">
         <v>5</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" ht="33" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14">
+      <c r="E8" s="10"/>
+      <c r="F8" s="16">
         <v>6</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" ht="33" spans="1:7">
-      <c r="A9" s="11"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14">
+      <c r="E9" s="10"/>
+      <c r="F9" s="16">
         <v>7</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" ht="16.5" spans="1:7">
-      <c r="A10" s="11"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="14">
+      <c r="E10" s="10"/>
+      <c r="F10" s="16">
         <v>8</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" ht="16.5" spans="1:7">
-      <c r="A11" s="11"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14">
+      <c r="E11" s="10"/>
+      <c r="F11" s="16">
         <v>9</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" ht="17.25" spans="1:7">
-      <c r="A12" s="16"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="27">
+      <c r="A12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="29">
         <v>10</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" ht="17.25" spans="1:7">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="15" ht="18" spans="1:7">
       <c r="A15" s="1" t="s">
@@ -1822,164 +1964,164 @@
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10">
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11">
         <v>1</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" ht="33" spans="1:7">
-      <c r="A18" s="11"/>
-      <c r="B18" s="35" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="14">
+      <c r="E18" s="10"/>
+      <c r="F18" s="16">
         <v>2</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" ht="16.5" spans="1:7">
-      <c r="A19" s="11"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="14">
+      <c r="D19" s="15"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="16">
         <v>3</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" ht="17.25" spans="1:7">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="14">
+      <c r="A20" s="17"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="16">
         <v>4</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="21" ht="17.25" spans="1:7">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="14">
+      <c r="A21" s="21"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="16">
         <v>5</v>
       </c>
-      <c r="G21" s="12"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" ht="33" spans="1:7">
       <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="14">
+      <c r="D22" s="15"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="16">
         <v>6</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" ht="16.5" spans="1:7">
-      <c r="A23" s="11"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="14">
+      <c r="D23" s="15"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="16">
         <v>7</v>
       </c>
-      <c r="G23" s="12"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" ht="16.5" spans="1:7">
-      <c r="A24" s="11"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="14">
+      <c r="D24" s="15"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="16">
         <v>8</v>
       </c>
-      <c r="G24" s="12"/>
+      <c r="G24" s="15"/>
     </row>
     <row r="25" ht="16.5" spans="1:7">
-      <c r="A25" s="11"/>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="14">
+      <c r="D25" s="15"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="16">
         <v>9</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" ht="17.25" spans="1:7">
-      <c r="A26" s="16"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="27">
+      <c r="A26" s="17"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="29">
         <v>10</v>
       </c>
-      <c r="G26" s="26"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" ht="17.25" spans="1:7">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="29" ht="18" spans="1:7">
       <c r="A29" s="1" t="s">
@@ -2017,156 +2159,156 @@
       <c r="A31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10">
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11">
         <v>1</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G31" s="38" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="32" ht="16.5" spans="1:7">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="12"/>
+      <c r="B32" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="14">
+      <c r="D32" s="15"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="16">
         <v>2</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="33" ht="16.5" spans="1:7">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="12"/>
+      <c r="B33" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="14">
+      <c r="D33" s="15"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="16">
         <v>3</v>
       </c>
-      <c r="G33" s="38" t="s">
+      <c r="G33" s="40" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="34" ht="17.25" spans="1:7">
-      <c r="A34" s="16"/>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="17"/>
+      <c r="B34" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="14">
+      <c r="D34" s="20"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="16">
         <v>4</v>
       </c>
-      <c r="G34" s="12"/>
+      <c r="G34" s="15"/>
     </row>
     <row r="35" ht="17.25" spans="1:7">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="14">
+      <c r="A35" s="21"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="16">
         <v>5</v>
       </c>
-      <c r="G35" s="12"/>
+      <c r="G35" s="15"/>
     </row>
     <row r="36" ht="17.25" spans="1:7">
       <c r="A36" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="14">
+      <c r="D36" s="15"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="16">
         <v>6</v>
       </c>
-      <c r="G36" s="12"/>
+      <c r="G36" s="15"/>
     </row>
     <row r="37" ht="16.5" spans="1:7">
-      <c r="A37" s="11"/>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="12"/>
+      <c r="B37" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="14">
+      <c r="D37" s="15"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="16">
         <v>7</v>
       </c>
-      <c r="G37" s="12"/>
+      <c r="G37" s="15"/>
     </row>
     <row r="38" ht="16.5" spans="1:7">
-      <c r="A38" s="11"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="14">
+      <c r="A38" s="12"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="16">
         <v>8</v>
       </c>
-      <c r="G38" s="12"/>
+      <c r="G38" s="15"/>
     </row>
     <row r="39" ht="16.5" spans="1:7">
-      <c r="A39" s="11"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="14">
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="16">
         <v>9</v>
       </c>
-      <c r="G39" s="12"/>
+      <c r="G39" s="15"/>
     </row>
     <row r="40" ht="17.25" spans="1:7">
-      <c r="A40" s="16"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="27">
+      <c r="A40" s="17"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="29">
         <v>10</v>
       </c>
-      <c r="G40" s="26"/>
+      <c r="G40" s="28"/>
     </row>
     <row r="41" ht="17.25" spans="1:7">
-      <c r="A41" s="28"/>
-      <c r="B41" s="29" t="s">
+      <c r="A41" s="30"/>
+      <c r="B41" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
     </row>
     <row r="43" ht="18" spans="1:7">
       <c r="A43" s="1" t="s">
@@ -2200,159 +2342,380 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" ht="17.25" spans="1:7">
+    <row r="45" ht="16.5" spans="1:7">
       <c r="A45" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="10">
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="11">
         <v>1</v>
       </c>
-      <c r="G45" s="7"/>
-    </row>
-    <row r="46" ht="16.5" spans="1:7">
-      <c r="A46" s="11"/>
-      <c r="B46" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="14">
+      <c r="G45" s="38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" ht="33.75" spans="1:7">
+      <c r="A46" s="12"/>
+      <c r="B46" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="10"/>
+      <c r="F46" s="16">
         <v>2</v>
       </c>
-      <c r="G46" s="12"/>
+      <c r="G46" s="15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="47" ht="33.75" spans="1:7">
-      <c r="A47" s="11"/>
-      <c r="B47" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="13" t="s">
+      <c r="A47" s="12"/>
+      <c r="B47" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="14">
+      <c r="D47" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="10"/>
+      <c r="F47" s="16">
         <v>3</v>
       </c>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" ht="33.75" spans="1:7">
-      <c r="A48" s="16"/>
-      <c r="B48" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="14">
+      <c r="G47" s="15"/>
+    </row>
+    <row r="48" ht="17.25" spans="1:7">
+      <c r="A48" s="17"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="16">
         <v>4</v>
       </c>
-      <c r="G48" s="12"/>
+      <c r="G48" s="15"/>
     </row>
     <row r="49" ht="17.25" spans="1:7">
-      <c r="A49" s="20"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="14">
+      <c r="A49" s="21"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="16">
         <v>5</v>
       </c>
-      <c r="G49" s="12"/>
+      <c r="G49" s="15"/>
     </row>
     <row r="50" ht="33" spans="1:7">
       <c r="A50" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="14">
+      <c r="B50" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" s="10"/>
+      <c r="F50" s="16">
         <v>6</v>
       </c>
-      <c r="G50" s="12"/>
-    </row>
-    <row r="51" ht="16.5" spans="1:7">
-      <c r="A51" s="11"/>
-      <c r="B51" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="14">
+      <c r="G50" s="15"/>
+    </row>
+    <row r="51" ht="17.25" spans="1:7">
+      <c r="A51" s="12"/>
+      <c r="B51" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51" s="10"/>
+      <c r="F51" s="16">
         <v>7</v>
       </c>
-      <c r="G51" s="12"/>
+      <c r="G51" s="15"/>
     </row>
     <row r="52" ht="16.5" spans="1:7">
-      <c r="A52" s="11"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="14">
+      <c r="A52" s="12"/>
+      <c r="B52" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="16">
         <v>8</v>
       </c>
-      <c r="G52" s="12"/>
+      <c r="G52" s="15"/>
     </row>
     <row r="53" ht="16.5" spans="1:7">
-      <c r="A53" s="11"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="14">
+      <c r="A53" s="12"/>
+      <c r="B53" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="15"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="16">
         <v>9</v>
       </c>
-      <c r="G53" s="12"/>
+      <c r="G53" s="15"/>
     </row>
     <row r="54" ht="17.25" spans="1:7">
-      <c r="A54" s="16"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="27">
+      <c r="A54" s="17"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="29">
         <v>10</v>
       </c>
-      <c r="G54" s="26"/>
+      <c r="G54" s="28"/>
     </row>
     <row r="55" ht="17.25" spans="1:7">
-      <c r="A55" s="28"/>
-      <c r="B55" s="29" t="s">
+      <c r="A55" s="30"/>
+      <c r="B55" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="31"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="33"/>
+    </row>
+    <row r="57" ht="18" spans="1:7">
+      <c r="A57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" ht="21.75" spans="1:7">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="5"/>
+      <c r="F58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" ht="16.5" spans="1:7">
+      <c r="A59" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="11">
+        <v>1</v>
+      </c>
+      <c r="G59" s="38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" ht="16.5" spans="1:7">
+      <c r="A60" s="12"/>
+      <c r="B60" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="15"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="16">
+        <v>2</v>
+      </c>
+      <c r="G60" s="40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" ht="16.5" spans="1:7">
+      <c r="A61" s="12"/>
+      <c r="B61" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="15"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="16">
+        <v>3</v>
+      </c>
+      <c r="G61" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" ht="17.25" spans="1:7">
+      <c r="A62" s="17"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="16">
+        <v>4</v>
+      </c>
+      <c r="G62" s="40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" ht="17.25" spans="1:7">
+      <c r="A63" s="21"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="16">
+        <v>5</v>
+      </c>
+      <c r="G63" s="40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" ht="16.5" spans="1:7">
+      <c r="A64" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="16">
+        <v>6</v>
+      </c>
+      <c r="G64" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" ht="16.5" spans="1:7">
+      <c r="A65" s="12"/>
+      <c r="B65" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" s="15"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="16">
+        <v>7</v>
+      </c>
+      <c r="G65" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" ht="16.5" spans="1:7">
+      <c r="A66" s="12"/>
+      <c r="B66" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D66" s="15"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="16">
+        <v>8</v>
+      </c>
+      <c r="G66" s="40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" ht="16.5" spans="1:7">
+      <c r="A67" s="12"/>
+      <c r="B67" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="16">
+        <v>9</v>
+      </c>
+      <c r="G67" s="40"/>
+    </row>
+    <row r="68" ht="17.25" spans="1:7">
+      <c r="A68" s="17"/>
+      <c r="B68" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D68" s="28"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="29">
+        <v>10</v>
+      </c>
+      <c r="G68" s="42"/>
+    </row>
+    <row r="69" ht="17.25" spans="1:7">
+      <c r="A69" s="30"/>
+      <c r="B69" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="25">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="B13:G13"/>
@@ -2365,6 +2728,9 @@
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="B55:G55"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="B69:G69"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A17:A20"/>
@@ -2373,6 +2739,8 @@
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A64:A68"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2385,8 +2753,251 @@
   <sheetPr/>
   <dimension ref="A1:G13"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="33.25" customWidth="1"/>
+    <col min="5" max="5" width="6.75" customWidth="1"/>
+    <col min="7" max="7" width="35.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" ht="21.75" spans="1:7">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" ht="16.5" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" ht="66" spans="1:7">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" ht="16.5" spans="1:7">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="16">
+        <v>3</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" ht="17.25" spans="1:7">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" ht="17.25" spans="1:7">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="16">
+        <v>5</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" ht="99" spans="1:7">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="16">
+        <v>6</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" ht="33" spans="1:7">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="16">
+        <v>7</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" ht="33" spans="1:7">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="16">
+        <v>8</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" ht="16.5" spans="1:7">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="16">
+        <v>9</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" ht="17.25" spans="1:7">
+      <c r="A12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="29">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="13" ht="17.25" spans="1:7">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A8:A12"/>
+  </mergeCells>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G13"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B13" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -2400,14 +3011,14 @@
   <sheetData>
     <row r="1" ht="18" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -2436,124 +3047,124 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10">
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" ht="16.5" spans="1:7">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="14">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="16">
         <v>2</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" ht="16.5" spans="1:7">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="14">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="16">
         <v>3</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" ht="17.25" spans="1:7">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="14">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16">
         <v>4</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" ht="17.25" spans="1:7">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="14">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="16">
         <v>5</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" ht="16.5" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="16">
         <v>6</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" ht="16.5" spans="1:7">
-      <c r="A9" s="11"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="16">
         <v>7</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" ht="16.5" spans="1:7">
-      <c r="A10" s="11"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="14">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="16">
         <v>8</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" ht="16.5" spans="1:7">
-      <c r="A11" s="11"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="16">
         <v>9</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" ht="17.25" spans="1:7">
-      <c r="A12" s="16"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="27">
+      <c r="A12" s="17"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="29">
         <v>10</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" ht="17.25" spans="1:7">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>